<commit_message>
Nulls handled in Node.Js code, error throw to client side.
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Reservations" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
   <si>
     <t>Book a Room</t>
   </si>
@@ -807,35 +807,10 @@
     <t>http://localhost:3000/api/reservations/1</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:3000/api/reservations/
-{
- "guest_id":"1",
- "date_of_arrival": "07/10/2018",
-   "date_of_departure": "07/20/2018",
-   "no_of_people":"99",
-    "reservation_comments": "99 ppl are coming",
-    "reservation_type_id":"1",
-   "sanskara_id":"1",
-   "is_a_reference": "0",
-  "advance_reminder_on":null
-} </t>
-  </si>
-  <si>
     <t>CALL sp_InsertGuestDetails('FirstName', 'Last Name', 'someone@gmail.com', '888', 'Besant Nagar', 'Chennai', '00', 'T N', 77);</t>
   </si>
   <si>
     <t>CALL sp_UpdateGuestDetails(4, 'FirstName', 'Last Name', 'someone@gmail.com', '888', 'Besant Nagar', 'Chennai', '00', 'T N', 77);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://localhost:3000/api/reservations/
-{
- "reservation_id":"1",
- "date_of_arrival": "07/10/2018",
-   "date_of_departure": "07/20/2018",
-   "no_of_people":"99",
-    "reservation_comments": "99 ppl are coming",
-  "advance_reminder_on":null
-} </t>
   </si>
   <si>
     <t>http://localhost:3000/api/econtacts/1</t>
@@ -920,6 +895,73 @@
   </si>
   <si>
     <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>Email ID allows null</t>
+  </si>
+  <si>
+    <t>CALL sp_InsertReservationDetails(5,'2018-06-11','2018-06-15',11,'11 ppl are coming',1,1,0, null);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:3000/api/reservations/
+{
+  "guest_id" : 5,
+  "date_of_arrival": "2018-06-11",
+   "date_of_departure": "2018-06-15",
+   "no_of_people":"8",
+    "reservation_comments": "test",
+    "reservation_type_id":"1",
+   "sanskara_id": null,
+   "is_a_reference": null,
+  "advance_reminder_on":"2018-06-01"
+} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:3000/api/reservations/5
+{
+  "date_of_arrival": "2018-06-20",
+  "date_of_departure": "2018-06-25",
+  "no_of_people":"88",
+  "reservation_comments": "test again",
+  "advance_reminder_on": null
+} </t>
+  </si>
+  <si>
+    <t>Even though reservation_comments, and advance_reminder_on are nullable columns, please pass existing data again to API call even if there are no changes.</t>
+  </si>
+  <si>
+    <t>Email ID allows null
+Even though email_id is nullable column, please pass existing data again to API call even if there is no change.</t>
+  </si>
+  <si>
+    <t>If no record is returned, it needs to be handled in client side</t>
+  </si>
+  <si>
+    <t>sp_CancelRoomBookings</t>
+  </si>
+  <si>
+    <t>reservation_id INT(6),
+room_booking_ids VARCHAR(400)</t>
+  </si>
+  <si>
+    <t>Called internally as of now</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For now, rooms also get cancelled when reservation is cancelled. Specific room cancellation needs to be handled.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Multiple IDs need to be handled for room bookings!</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1574,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="62" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,7 +1685,9 @@
       <c r="G2" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="I2" s="17" t="s">
         <v>3</v>
       </c>
@@ -1668,9 +1712,11 @@
         <v>148</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="I3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1695,9 +1741,11 @@
         <v>149</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="I4" s="17" t="s">
         <v>3</v>
       </c>
@@ -1746,17 +1794,17 @@
         <v>110</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>91</v>
+        <v>174</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1773,12 +1821,14 @@
         <v>110</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="I7" t="s">
         <v>3</v>
       </c>
@@ -1800,7 +1850,7 @@
         <v>109</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>98</v>
@@ -1827,10 +1877,10 @@
         <v>110</v>
       </c>
       <c r="F9" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="17"/>
@@ -1852,10 +1902,10 @@
         <v>110</v>
       </c>
       <c r="F10" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="17" t="s">
@@ -1882,10 +1932,10 @@
         <v>150</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>12</v>
@@ -1911,13 +1961,10 @@
         <v>151</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1934,17 +1981,15 @@
         <v>55</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>66</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="H13" s="16"/>
       <c r="I13" s="17" t="s">
         <v>3</v>
       </c>
@@ -1966,12 +2011,12 @@
         <v>109</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="I14" s="17" t="s">
@@ -1995,10 +2040,10 @@
         <v>110</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>73</v>
@@ -2014,47 +2059,61 @@
       <c r="D16" s="47"/>
       <c r="E16" s="47"/>
       <c r="F16" s="27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H16" s="48"/>
       <c r="I16" s="49"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="F17" s="48"/>
+      <c r="H17" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="45" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="45"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
@@ -2064,13 +2123,13 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F12" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3" display="http://localhost:3000/api/reservations/_x000a__x000a__x000a__x000a_{_x000a_ &quot;guest_id&quot;:&quot;1&quot;,_x000a_ &quot;date_of_arrival&quot;: &quot;07/10/2018&quot;,_x000a_   &quot;date_of_departure&quot;: &quot;07/20/2018&quot;,_x000a_   &quot;no_of_people&quot;:&quot;99&quot;,_x000a_    &quot;reservation_comments&quot;: &quot;99 ppl are coming&quot;,_x000a_    &quot;reservation_type_id&quot;:&quot;1&quot;,_x000a_   &quot;sanskara_id&quot;:&quot;1&quot;,_x000a_   &quot;is_a_reference&quot;: &quot;0&quot;,_x000a_  &quot;advance_reminder_on&quot;:null_x000a_} "/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F9" r:id="rId5"/>
-    <hyperlink ref="F13" r:id="rId6"/>
-    <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F15" r:id="rId8"/>
-    <hyperlink ref="F16" r:id="rId9"/>
+    <hyperlink ref="F9" r:id="rId3"/>
+    <hyperlink ref="F13" r:id="rId4"/>
+    <hyperlink ref="F11" r:id="rId5"/>
+    <hyperlink ref="F15" r:id="rId6"/>
+    <hyperlink ref="F16" r:id="rId7"/>
+    <hyperlink ref="F6" r:id="rId8" display="http://localhost:3000/api/reservations/_x000a__x000a_{_x000a_  &quot;guest_id&quot; : 5,_x000a_  &quot;date_of_arrival&quot;: &quot;2018-06-11&quot;,_x000a_   &quot;date_of_departure&quot;: &quot;2018-06-15&quot;,_x000a_   &quot;no_of_people&quot;:&quot;8&quot;,_x000a_    &quot;reservation_comments&quot;: &quot;test&quot;,_x000a_    &quot;reservation_type_id&quot;:&quot;1&quot;,_x000a_   &quot;sanskara_id&quot;: null,_x000a_   &quot;is_a_reference&quot;: null,_x000a_  &quot;advance_reminder_on&quot;:&quot;2018-06-01&quot;_x000a_} "/>
+    <hyperlink ref="F7" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2081,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2313,7 +2372,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2598,7 +2657,7 @@
     </row>
     <row r="24" spans="1:7" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Node.Js to return values to client side
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhatm\Desktop\PN Reservations System\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhatm\Documents\GitHub\parmarth-niketan\Docs\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reservations" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="190">
   <si>
     <t>Book a Room</t>
   </si>
@@ -566,50 +566,6 @@
     <t>http://localhost:3000/api/checkouts/</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">If entire reservation is checking in, pass reservation_id alone. Else if partial checkin, pass room_booking_id
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Multiple IDs not working!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If entire reservation is checking in, pass reservation_id alone. Else if partial checkin, pass room_booking_id
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Multiple IDs not working!
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bill amount must be generated and shown</t>
-    </r>
-  </si>
-  <si>
     <t>None???</t>
   </si>
   <si>
@@ -947,28 +903,53 @@
     <t>Called internally as of now</t>
   </si>
   <si>
+    <t>If entire reservation is checking in, pass reservation_id alone. Else if partial checkin, pass room_booking_id</t>
+  </si>
+  <si>
+    <t>CALL sp_UpdateTodaysCheckIns('1,2,3','5,6');</t>
+  </si>
+  <si>
+    <t>For now, rooms also get cancelled when reservation is cancelled. Specific room cancellation needs to be handled.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">For now, rooms also get cancelled when reservation is cancelled. Specific room cancellation needs to be handled.
-</t>
+      <t>If entire reservation is checking in, pass reservation_id alone. Else if partial checkin, pass room_booking_id</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Multiple IDs need to be handled for room bookings!</t>
+      <t/>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL sp_UpdateDonationDetails(null, 1,1,'2018-05-26',5000,'R123',0);
+</t>
+  </si>
+  <si>
+    <t>Same SP used in Edit Reservations page. 
+is_advance = 0
+Even if partial check out, send reservation_id, guest_id from front end</t>
+  </si>
+  <si>
+    <t>sp_GetBookingsCheckOutTotal</t>
+  </si>
+  <si>
+    <t>total DECIMAL(10,0)</t>
+  </si>
+  <si>
+    <t>CALL sp_GetBookingsCheckOutTotal('2,1');</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1029,14 +1010,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1044,7 +1017,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1087,6 +1060,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1123,7 +1108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1228,9 +1213,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1253,18 +1235,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1618,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A13" zoomScale="65" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1648,7 +1639,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>99</v>
@@ -1659,7 +1650,7 @@
       <c r="H1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="43" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1671,22 +1662,22 @@
         <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="40" t="s">
-        <v>147</v>
+      <c r="F2" s="39" t="s">
+        <v>145</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>3</v>
@@ -1700,7 +1691,7 @@
         <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>95</v>
@@ -1709,13 +1700,13 @@
         <v>110</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>12</v>
@@ -1729,7 +1720,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>55</v>
@@ -1738,13 +1729,13 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>3</v>
@@ -1758,16 +1749,16 @@
         <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>152</v>
+      <c r="F5" s="40" t="s">
+        <v>150</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>92</v>
@@ -1785,19 +1776,19 @@
         <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="3" t="s">
@@ -1812,7 +1803,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>55</v>
@@ -1821,13 +1812,13 @@
         <v>110</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>93</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I7" t="s">
         <v>3</v>
@@ -1841,16 +1832,16 @@
         <v>79</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="41" t="s">
-        <v>155</v>
+      <c r="F8" s="40" t="s">
+        <v>153</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>98</v>
@@ -1868,7 +1859,7 @@
         <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>55</v>
@@ -1876,11 +1867,11 @@
       <c r="E9" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="17"/>
@@ -1893,7 +1884,7 @@
         <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>55</v>
@@ -1902,10 +1893,10 @@
         <v>110</v>
       </c>
       <c r="F10" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="17" t="s">
@@ -1923,19 +1914,19 @@
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="40" t="s">
-        <v>150</v>
+      <c r="F11" s="39" t="s">
+        <v>148</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>12</v>
@@ -1952,19 +1943,19 @@
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>151</v>
+      <c r="F12" s="41" t="s">
+        <v>149</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1981,13 +1972,13 @@
         <v>55</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>163</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="17" t="s">
@@ -2005,16 +1996,16 @@
         <v>75</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="41" t="s">
-        <v>167</v>
+      <c r="F14" s="40" t="s">
+        <v>165</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>20</v>
@@ -2024,26 +2015,26 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="46">
+      <c r="A15" s="50">
         <v>14</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="47" t="s">
+      <c r="C15" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="51" t="s">
         <v>110</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>73</v>
@@ -2053,32 +2044,32 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H16" s="48"/>
       <c r="I16" s="49"/>
     </row>
     <row r="17" spans="2:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F17" s="48"/>
       <c r="H17" s="1" t="s">
@@ -2089,10 +2080,10 @@
       <c r="B18" s="2"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="C23" s="45"/>
+      <c r="B23" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="44"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
@@ -2126,10 +2117,10 @@
     <hyperlink ref="F9" r:id="rId3"/>
     <hyperlink ref="F13" r:id="rId4"/>
     <hyperlink ref="F11" r:id="rId5"/>
-    <hyperlink ref="F15" r:id="rId6"/>
-    <hyperlink ref="F16" r:id="rId7"/>
-    <hyperlink ref="F6" r:id="rId8" display="http://localhost:3000/api/reservations/_x000a__x000a_{_x000a_  &quot;guest_id&quot; : 5,_x000a_  &quot;date_of_arrival&quot;: &quot;2018-06-11&quot;,_x000a_   &quot;date_of_departure&quot;: &quot;2018-06-15&quot;,_x000a_   &quot;no_of_people&quot;:&quot;8&quot;,_x000a_    &quot;reservation_comments&quot;: &quot;test&quot;,_x000a_    &quot;reservation_type_id&quot;:&quot;1&quot;,_x000a_   &quot;sanskara_id&quot;: null,_x000a_   &quot;is_a_reference&quot;: null,_x000a_  &quot;advance_reminder_on&quot;:&quot;2018-06-01&quot;_x000a_} "/>
-    <hyperlink ref="F7" r:id="rId9"/>
+    <hyperlink ref="F16" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7" display="http://localhost:3000/api/reservations/_x000a__x000a_{_x000a_  &quot;guest_id&quot; : 5,_x000a_  &quot;date_of_arrival&quot;: &quot;2018-06-11&quot;,_x000a_   &quot;date_of_departure&quot;: &quot;2018-06-15&quot;,_x000a_   &quot;no_of_people&quot;:&quot;8&quot;,_x000a_    &quot;reservation_comments&quot;: &quot;test&quot;,_x000a_    &quot;reservation_type_id&quot;:&quot;1&quot;,_x000a_   &quot;sanskara_id&quot;: null,_x000a_   &quot;is_a_reference&quot;: null,_x000a_  &quot;advance_reminder_on&quot;:&quot;2018-06-01&quot;_x000a_} "/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -2138,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2192,12 +2183,12 @@
         <v>55</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="42" t="s">
         <v>119</v>
       </c>
       <c r="G2" s="31" t="s">
@@ -2218,12 +2209,12 @@
         <v>55</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>120</v>
       </c>
       <c r="G3" s="31" t="s">
@@ -2237,26 +2228,26 @@
       <c r="A4" s="29">
         <v>3</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="33" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>105</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>118</v>
+        <v>182</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>122</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
@@ -2270,12 +2261,12 @@
         <v>55</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>121</v>
       </c>
       <c r="G5" s="31" t="s">
@@ -2293,22 +2284,22 @@
         <v>43</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>107</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>118</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
@@ -2322,12 +2313,12 @@
         <v>55</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>111</v>
       </c>
       <c r="G7" s="31" t="s">
@@ -2345,25 +2336,75 @@
       <c r="C8" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="37" t="s">
+      <c r="D8" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="37" t="s">
         <v>114</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="34" t="s">
-        <v>62</v>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>8</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="47"/>
+      <c r="G9" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>9</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2401,7 +2442,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F1" s="28" t="s">
         <v>99</v>
@@ -2421,18 +2462,18 @@
         <v>69</v>
       </c>
       <c r="C2" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>103</v>
       </c>
       <c r="H2" s="32"/>
@@ -2448,18 +2489,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>101</v>
       </c>
       <c r="H3" s="32" t="s">
@@ -2657,7 +2698,7 @@
     </row>
     <row r="24" spans="1:7" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit with Dashboard (individual components only work)
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -677,16 +677,6 @@
 count</t>
   </si>
   <si>
-    <t>reservation_id INT(6), 
-reservation_type_id TINYINT(4), 
-first_name VARCHAR(45),  
-last_name VARCHAR(45), 
-room_booking_id INT(6), 
-room_no VARCHAR(10), 
-rooms.floor_no TINYINT(4), 
-rooms.block_id TINYINT(4)</t>
-  </si>
-  <si>
     <t>room_booking_id INT(6), 
 room_no VARCHAR(10)</t>
   </si>
@@ -943,6 +933,15 @@
   </si>
   <si>
     <t>CALL sp_GetBookingsCheckOutTotal('2,1');</t>
+  </si>
+  <si>
+    <t>reservation_id INT(6), 
+reservation_type_id TINYINT(4), 
+first_name VARCHAR(45),  
+last_name VARCHAR(45), 
+room_booking_id INT(6), 
+room_no VARCHAR(10), 
+rooms.block_id TINYINT(4)</t>
   </si>
 </sst>
 </file>
@@ -1671,13 +1670,13 @@
         <v>109</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>3</v>
@@ -1700,13 +1699,13 @@
         <v>110</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>12</v>
@@ -1729,13 +1728,13 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>3</v>
@@ -1758,7 +1757,7 @@
         <v>109</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>92</v>
@@ -1785,10 +1784,10 @@
         <v>110</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="3" t="s">
@@ -1812,13 +1811,13 @@
         <v>110</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>93</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I7" t="s">
         <v>3</v>
@@ -1841,7 +1840,7 @@
         <v>109</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>98</v>
@@ -1868,10 +1867,10 @@
         <v>110</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="17"/>
@@ -1893,10 +1892,10 @@
         <v>110</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="17" t="s">
@@ -1920,13 +1919,13 @@
         <v>109</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>12</v>
@@ -1949,13 +1948,13 @@
         <v>109</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1972,13 +1971,13 @@
         <v>55</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="17" t="s">
@@ -2002,10 +2001,10 @@
         <v>109</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>20</v>
@@ -2031,10 +2030,10 @@
         <v>110</v>
       </c>
       <c r="F15" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="H15" s="48" t="s">
         <v>73</v>
@@ -2050,30 +2049,30 @@
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
       <c r="F16" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H16" s="48"/>
       <c r="I16" s="49"/>
     </row>
     <row r="17" spans="2:8" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F17" s="48"/>
       <c r="H17" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -2081,7 +2080,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" s="44"/>
     </row>
@@ -2132,7 +2131,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,7 +2197,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -2209,12 +2208,12 @@
         <v>55</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="E3" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="42" t="s">
         <v>120</v>
       </c>
       <c r="G3" s="31" t="s">
@@ -2232,7 +2231,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>122</v>
@@ -2244,13 +2243,13 @@
         <v>105</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="110.4" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -2261,7 +2260,7 @@
         <v>55</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="E5" s="36" t="s">
         <v>109</v>
@@ -2284,7 +2283,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>122</v>
@@ -2299,7 +2298,7 @@
         <v>118</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
@@ -2313,7 +2312,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>109</v>
@@ -2355,20 +2354,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>188</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>110</v>
       </c>
       <c r="F9" s="47"/>
       <c r="G9" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H9" s="34"/>
     </row>
@@ -2389,22 +2388,23 @@
         <v>110</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2462,10 +2462,10 @@
         <v>69</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>109</v>
@@ -2489,10 +2489,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" s="36" t="s">
         <v>109</v>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="24" spans="1:7" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dashboard Page Completed with minor issues open
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -2131,7 +2131,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2223,7 +2223,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="E4" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="42" t="s">
         <v>105</v>
       </c>
       <c r="G4" s="31" t="s">
@@ -2402,9 +2402,10 @@
     <hyperlink ref="F10" r:id="rId1"/>
     <hyperlink ref="F2" r:id="rId2"/>
     <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Dashboard, Reports, Google Auth (partial) completed
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reservations" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="191">
   <si>
     <t>Book a Room</t>
   </si>
@@ -942,6 +942,9 @@
 room_booking_id INT(6), 
 room_no VARCHAR(10), 
 rooms.block_id TINYINT(4)</t>
+  </si>
+  <si>
+    <t>sp_CleanupNoShow</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="65" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="B10" zoomScale="87" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2414,7 +2417,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2530,9 +2533,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2696,6 +2699,11 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="206.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">

</xml_diff>

<commit_message>
Lots of bug fixes and until Guest Contact CSS
</commit_message>
<xml_diff>
--- a/Docs/Database/Stored Procs.xlsx
+++ b/Docs/Database/Stored Procs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reservations" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="192">
   <si>
     <t>Book a Room</t>
   </si>
@@ -945,6 +945,9 @@
   </si>
   <si>
     <t>sp_CleanupNoShow</t>
+  </si>
+  <si>
+    <t>sp_SearchReservations</t>
   </si>
 </sst>
 </file>
@@ -2131,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,6 +2401,11 @@
       </c>
       <c r="H10" s="1" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2533,7 +2541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>

</xml_diff>